<commit_message>
new implementations and working fine
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -13,6 +13,56 @@
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>André</t>
+  </si>
+  <si>
+    <t>Maurício</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Marcelo</t>
+  </si>
+  <si>
+    <t>Jamile</t>
+  </si>
+  <si>
+    <t>Bryann</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Natália</t>
+  </si>
+  <si>
+    <t>Isabela</t>
+  </si>
+  <si>
+    <t>Luiz</t>
+  </si>
+  <si>
+    <t>Beatriz</t>
+  </si>
+  <si>
+    <t>Sandra</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>1234abcs</t>
+  </si>
+  <si>
+    <t>(11) 99447-9393abcd</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -389,75 +439,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>11994479393</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>119912962978</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>70548956</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>77232288</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
+        <v>1254</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>78569878</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>79265879</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>72123645</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>74897654</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>991296297</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>1191296297</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>12991296297</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>